<commit_message>
finish svm model running
</commit_message>
<xml_diff>
--- a/Results/SVM.xlsx
+++ b/Results/SVM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE64555-1798-F548-BA5D-D95F5A07A36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6B79F9-F05F-4B42-8507-F6E01F032BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,10 +1990,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$45:$D$52</c:f>
+              <c:f>Sheet1!$D$45:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1E-3</c:v>
                 </c:pt>
@@ -2013,9 +2013,15 @@
                   <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3.2000000000000001E-2</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>6.4000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2023,10 +2029,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$45:$E$52</c:f>
+              <c:f>Sheet1!$E$45:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.71700051361068295</c:v>
                 </c:pt>
@@ -2049,6 +2055,12 @@
                   <c:v>0.72213662044170501</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.72213662044170501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72213662044170501</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.72213662044170501</c:v>
                 </c:pt>
               </c:numCache>
@@ -6068,10 +6080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+      <selection activeCell="E50" sqref="E50:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6618,7 +6630,7 @@
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D51">
-        <v>3.2000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E51">
         <v>0.72213662044170501</v>
@@ -6626,9 +6638,25 @@
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D52">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E52">
+        <v>0.72213662044170501</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E53">
+        <v>0.72213662044170501</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D54">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="E52">
+      <c r="E54">
         <v>0.72213662044170501</v>
       </c>
     </row>

</xml_diff>